<commit_message>
adding nichole to day 2 panel
</commit_message>
<xml_diff>
--- a/docs/events2.xlsx
+++ b/docs/events2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thema\git\difa-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98E1C02B-DDE3-4CE7-91D1-BAE4C81D6FEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A38D65B7-55E0-4E44-B75C-021DE02C0F57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33240" yWindow="2025" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4635" yWindow="2655" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -108,9 +108,6 @@
     <t>5:00PM</t>
   </si>
   <si>
-    <t>[Wen You](https://med.virginia.edu/phs/2019/08/01/you-wen/), [Bruce Weinberg](https://economics.osu.edu/people/weinberg.27), [Mark Prell](https://www.ers.usda.gov/authors/ers-staff-directory/mark-prell/)</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -145,6 +142,9 @@
   </si>
   <si>
     <t>[Lauren Chenarides](https://dataifa.github.io/difa-project/lauren_chenarides.html)</t>
+  </si>
+  <si>
+    <t>[Wen You](https://med.virginia.edu/phs/2019/08/01/you-wen/), [Nichole Szembrot](https://sites.google.com/site/nicholeszembrot/), [Mark Prell](https://www.ers.usda.gov/authors/ers-staff-directory/mark-prell/), [Bruce Weinberg](https://economics.osu.edu/people/weinberg.27)</t>
   </si>
 </sst>
 </file>
@@ -469,7 +469,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,7 +496,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -516,10 +516,10 @@
         <v>4</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -536,10 +536,10 @@
         <v>5</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -559,7 +559,7 @@
         <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -596,10 +596,10 @@
         <v>9</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -616,10 +616,10 @@
         <v>10</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -636,10 +636,10 @@
         <v>11</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -656,10 +656,10 @@
         <v>12</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more little comingsoon detail work
</commit_message>
<xml_diff>
--- a/docs/events2.xlsx
+++ b/docs/events2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thema\git\difa-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CD559AC-A3AF-47EC-8537-CFDB5F45973A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C895BC8F-0D6C-4DB8-9EED-0B96285A376E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15240" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
   <si>
     <t>Start Time</t>
   </si>
@@ -139,9 +139,6 @@
   </si>
   <si>
     <t>[Lauren Chenarides](https://dataifa.github.io/difa-project/lauren_chenarides.html)</t>
-  </si>
-  <si>
-    <t>https://dataifa.github.io/difa-project/comingsoon.html</t>
   </si>
   <si>
     <t>[Wen You](https://dataifa.github.io/difa-project/comingsoon.html), [Nichole Szembrot](https://dataifa.github.io/difa-project/comingsoon.html), [Mark Prell]https://dataifa.github.io/difa-project/comingsoon.html), [Bruce Weinberg](https://dataifa.github.io/difa-project/comingsoon.html)</t>
@@ -482,8 +479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,7 +550,7 @@
         <v>29</v>
       </c>
       <c r="F3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -573,7 +570,7 @@
         <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -677,14 +674,9 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D13" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="D13" s="3"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D13" r:id="rId1" xr:uid="{69E48953-1A94-476F-A09B-117BDC467516}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
even more detail work!
</commit_message>
<xml_diff>
--- a/docs/events2.xlsx
+++ b/docs/events2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thema\git\difa-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C895BC8F-0D6C-4DB8-9EED-0B96285A376E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F855AB52-6D13-411A-A944-90E4C853EBAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -141,10 +141,10 @@
     <t>[Lauren Chenarides](https://dataifa.github.io/difa-project/lauren_chenarides.html)</t>
   </si>
   <si>
-    <t>[Wen You](https://dataifa.github.io/difa-project/comingsoon.html), [Nichole Szembrot](https://dataifa.github.io/difa-project/comingsoon.html), [Mark Prell]https://dataifa.github.io/difa-project/comingsoon.html), [Bruce Weinberg](https://dataifa.github.io/difa-project/comingsoon.html)</t>
-  </si>
-  <si>
     <t>[George Davis](https://dataifa.github.io/difa-project/george_davis.html), [Joe Cummins](https://dataifa.github.io/difa-project/comingsoon.html)</t>
+  </si>
+  <si>
+    <t>[Wen You](https://dataifa.github.io/difa-project/comingsoon.html), [Nichole Szembrot](https://dataifa.github.io/difa-project/comingsoon.html), [Mark Prell](https://dataifa.github.io/difa-project/comingsoon.html), [Bruce Weinberg](https://dataifa.github.io/difa-project/comingsoon.html)</t>
   </si>
 </sst>
 </file>
@@ -479,8 +479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,7 +550,7 @@
         <v>29</v>
       </c>
       <c r="F3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -570,7 +570,7 @@
         <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
changing activity page, adding matt bombyk
</commit_message>
<xml_diff>
--- a/docs/events2.xlsx
+++ b/docs/events2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thema\git\difa-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAED687B-3D87-4602-9689-EB383EFFD108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2A07B38-0796-4197-AFC3-1521B2A9F013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4410" yWindow="1905" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="45">
   <si>
     <t>Start Time</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Session 5</t>
   </si>
   <si>
-    <t>Session 6 (Research Presentations)</t>
-  </si>
-  <si>
     <t>Frontiers in evidence-based policymaking</t>
   </si>
   <si>
@@ -84,27 +81,12 @@
     <t>Duration</t>
   </si>
   <si>
-    <t>2:15PM</t>
-  </si>
-  <si>
     <t>60 Minutes</t>
   </si>
   <si>
-    <t>2:30PM</t>
-  </si>
-  <si>
-    <t>3:15PM</t>
-  </si>
-  <si>
     <t>45 minutes</t>
   </si>
   <si>
-    <t>4:00PM</t>
-  </si>
-  <si>
-    <t>4:45PM</t>
-  </si>
-  <si>
     <t>5:00PM</t>
   </si>
   <si>
@@ -145,6 +127,39 @@
   </si>
   <si>
     <t>[Wen You](https://dataifa.github.io/difa-project/wen_you.html), [Nichole Szembrot](https://dataifa.github.io/difa-project/comingsoon.html), [Mark Prell](https://dataifa.github.io/difa-project/comingsoon.html), [Bruce Weinberg](https://dataifa.github.io/difa-project/bruce_weinberg.html)</t>
+  </si>
+  <si>
+    <t>1:35PM</t>
+  </si>
+  <si>
+    <t>20 minutes</t>
+  </si>
+  <si>
+    <t>Session 6</t>
+  </si>
+  <si>
+    <t>Linking Administrative Data: The IPUMS Experience</t>
+  </si>
+  <si>
+    <t>[Matt Bombyk](https://dataifa.github.io/difa-project/comingsoon.html)</t>
+  </si>
+  <si>
+    <t>2:35PM</t>
+  </si>
+  <si>
+    <t>Session 7 (Research Presentations)</t>
+  </si>
+  <si>
+    <t>2:50PM</t>
+  </si>
+  <si>
+    <t>3:30PM</t>
+  </si>
+  <si>
+    <t>4:10PM</t>
+  </si>
+  <si>
+    <t>4:50PM</t>
   </si>
 </sst>
 </file>
@@ -477,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,13 +516,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -515,166 +530,186 @@
     </row>
     <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
         <v>7</v>
       </c>
-      <c r="F4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>30</v>
+      <c r="E6" t="s">
+        <v>7</v>
       </c>
       <c r="F6" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="F7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="F8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D13" s="3"/>
+      <c r="E10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D14" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>